<commit_message>
Fixing filtering log error
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2022_SedTraps_FilteringLog.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2022_SedTraps_FilteringLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/Virginia Tech/Sed Traps/2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/GitHub/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB01C59-48B6-AE47-87B3-352E1725A2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCFA2D2-4B45-6A40-A448-3806EDB51AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" activeTab="1" xr2:uid="{00E498B5-789D-C347-B985-BEE6B94CD0F9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{00E498B5-789D-C347-B985-BEE6B94CD0F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2374,13 +2374,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2705,9 +2705,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73323465-4FD0-CC47-9C8F-2D6D3D918D41}">
   <dimension ref="A1:L529"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J465" sqref="J465:J481"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E211" sqref="E211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9109,7 +9109,7 @@
         <v>0.96599999999999997</v>
       </c>
       <c r="E211" s="10">
-        <v>1.7000000000000001E-2</v>
+        <v>0.107</v>
       </c>
       <c r="F211" s="10">
         <v>0.124</v>
@@ -9122,7 +9122,7 @@
       </c>
       <c r="I211" s="1">
         <f t="shared" si="4"/>
-        <v>0.107</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="J211">
         <v>14</v>
@@ -18889,7 +18889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FCF045D-C554-7B47-B703-D61A53B17FEC}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -18942,7 +18942,7 @@
       <c r="K1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="19" t="s">
         <v>581</v>
       </c>
     </row>
@@ -26478,16 +26478,16 @@
       <c r="A65" s="4"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="19"/>
+      <c r="A66" s="20"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="20"/>
+      <c r="A67" s="21"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="19"/>
+      <c r="A68" s="20"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="20"/>
+      <c r="A69" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -27911,16 +27911,16 @@
       <c r="A73" s="4"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="19"/>
+      <c r="A74" s="20"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="20"/>
+      <c r="A75" s="21"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="19"/>
+      <c r="A76" s="20"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="20"/>
+      <c r="A77" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>